<commit_message>
Added cellulose option only
</commit_message>
<xml_diff>
--- a/SAPcalc.xlsx
+++ b/SAPcalc.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aa5c90c7b976d1c7/Documents/GitHub/PassiveHouse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SamRussell/Documents/GitHub/PassiveHouse/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{BA548996-6B57-48C3-B389-673B6A17FC7F}"/>
+    <workbookView xWindow="1280" yWindow="1340" windowWidth="23400" windowHeight="15680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,15 @@
     <definedName name="SAP2e">Sheet1!$B$6</definedName>
     <definedName name="SAP2n">Sheet1!$B$7</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -62,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,22 +427,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADE30C9-330B-46B3-A40C-8295ADD74717}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="22" max="22" width="8.88671875" style="1"/>
-    <col min="29" max="29" width="11.109375" customWidth="1"/>
-    <col min="37" max="37" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="8.83203125" style="1"/>
+    <col min="22" max="22" width="8.83203125" style="1"/>
+    <col min="29" max="29" width="11.1640625" customWidth="1"/>
+    <col min="37" max="37" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2">
+        <v>3</v>
+      </c>
       <c r="N1" s="2" t="s">
         <v>0</v>
       </c>
@@ -481,7 +496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -575,7 +590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>83.45</v>
       </c>
@@ -596,7 +611,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H6" si="0">G3+F3+E3</f>
+        <f t="shared" ref="H3" si="0">G3+F3+E3</f>
         <v>0</v>
       </c>
       <c r="I3">
@@ -658,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>87.2</v>
       </c>
@@ -732,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -802,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -879,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -948,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8">
         <f>SUM(A2:A7)</f>
         <v>170.65</v>
@@ -991,7 +1006,7 @@
         <v>400.18</v>
       </c>
       <c r="AC8">
-        <f t="shared" ref="AC7:AC18" si="10">AB8*Y8</f>
+        <f t="shared" ref="AC8:AC18" si="10">AB8*Y8</f>
         <v>1500.675</v>
       </c>
       <c r="AE8">
@@ -1014,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
       <c r="N9">
         <v>4.0999999999999996</v>
       </c>
@@ -1067,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="N10">
         <v>4.7</v>
       </c>
@@ -1130,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
       <c r="N11">
         <v>5</v>
       </c>
@@ -1185,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="N12">
         <v>5.2</v>
       </c>
@@ -1225,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
       <c r="N13">
         <v>5</v>
       </c>
@@ -1278,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="Y14">
         <v>0</v>
       </c>
@@ -1302,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
       <c r="Y15">
         <v>0</v>
       </c>
@@ -1314,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
       <c r="Y16">
         <v>246.11</v>
       </c>
@@ -1323,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="25:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="25:29" x14ac:dyDescent="0.2">
       <c r="Y17">
         <f>Y7</f>
         <v>83.45</v>
@@ -1336,7 +1351,7 @@
         <v>33395.021000000001</v>
       </c>
     </row>
-    <row r="18" spans="25:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="25:29" x14ac:dyDescent="0.2">
       <c r="Y18">
         <f>SAP1b+SAP1c</f>
         <v>170.65</v>
@@ -1346,31 +1361,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="25:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="25:29" x14ac:dyDescent="0.2">
       <c r="AC20">
         <f>SUM(AA2:AA11)+AA13</f>
         <v>79.142513488372089</v>
       </c>
     </row>
-    <row r="21" spans="25:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="25:29" x14ac:dyDescent="0.2">
       <c r="AC21">
         <f>SUM(AC6:AC11)+SUM(AC13:AC18)</f>
         <v>202323.00440000001</v>
       </c>
     </row>
-    <row r="22" spans="25:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="25:29" x14ac:dyDescent="0.2">
       <c r="AC22">
         <f>AC21/A8</f>
         <v>1185.6021353647818</v>
       </c>
     </row>
-    <row r="23" spans="25:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="25:29" x14ac:dyDescent="0.2">
       <c r="AC23">
         <f>0.15*Y12</f>
         <v>69.596999999999994</v>
       </c>
     </row>
-    <row r="24" spans="25:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="25:29" x14ac:dyDescent="0.2">
       <c r="AC24">
         <f>AC23+AC20</f>
         <v>148.7395134883721</v>

</xml_diff>